<commit_message>
Progress on controller firmware
</commit_message>
<xml_diff>
--- a/Mobitec_IDC_Connector.xlsx
+++ b/Mobitec_IDC_Connector.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdonze/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\flipdot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2330D898-305F-1345-BB86-8B0B8F99C6E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3048E7A-089D-435F-8862-3327DE0A94CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{0B4254AC-718B-3F48-B23B-062AC4C822A7}"/>
+    <workbookView xWindow="76680" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{0B4254AC-718B-3F48-B23B-062AC4C822A7}"/>
   </bookViews>
   <sheets>
     <sheet name="IDC pinout" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="78">
   <si>
     <t>Pin 1</t>
   </si>
@@ -256,6 +256,21 @@
   </si>
   <si>
     <t>CH13</t>
+  </si>
+  <si>
+    <t>Row address</t>
+  </si>
+  <si>
+    <t>Row high/low side</t>
+  </si>
+  <si>
+    <t>Column address</t>
+  </si>
+  <si>
+    <t>Column high/low side</t>
+  </si>
+  <si>
+    <t>Column section (panel select)</t>
   </si>
 </sst>
 </file>
@@ -285,7 +300,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,6 +325,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -323,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -332,6 +371,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,19 +701,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4177AF-D5C3-9E45-BE81-E57136F23079}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="38.5" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -666,7 +721,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -674,7 +729,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -682,7 +737,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -690,7 +745,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -698,84 +753,109 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -783,150 +863,195 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="9" t="s">
         <v>18</v>
       </c>
       <c r="C22" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C24" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C25" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="9" t="s">
         <v>30</v>
       </c>
       <c r="C26" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -935,6 +1060,13 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F26"/>
+    <mergeCell ref="D6:F10"/>
+    <mergeCell ref="D11:F12"/>
+    <mergeCell ref="D14:F18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -943,13 +1075,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22430D4-7B53-9A41-9562-E8CD56F70102}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -957,7 +1089,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -965,7 +1097,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -976,7 +1108,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -987,7 +1119,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -998,7 +1130,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1009,7 +1141,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -1020,7 +1152,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -1031,7 +1163,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1039,7 +1171,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1050,7 +1182,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -1061,7 +1193,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1072,7 +1204,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1083,7 +1215,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1094,7 +1226,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1105,7 +1237,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -1116,7 +1248,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>58</v>
       </c>

</xml_diff>